<commit_message>
[2017.01.23] SAM UML 추가 T/C 추가
</commit_message>
<xml_diff>
--- a/StoryAlbum/check_list.xlsx
+++ b/StoryAlbum/check_list.xlsx
@@ -7,8 +7,8 @@
     <workbookView xWindow="360" yWindow="30" windowWidth="25755" windowHeight="11595" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="잔여이슈" sheetId="1" r:id="rId1"/>
+    <sheet name="TC" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames/>
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="74">
   <si>
     <t>사진 찍고 back 키 시 찍었던 파일 모두 삭제 필요.</t>
   </si>
@@ -74,6 +74,174 @@
   </si>
   <si>
     <t>사진 확대 기능</t>
+  </si>
+  <si>
+    <t>DB</t>
+  </si>
+  <si>
+    <t>delete story thread로 처리</t>
+  </si>
+  <si>
+    <t>Story List</t>
+  </si>
+  <si>
+    <t>리스트</t>
+  </si>
+  <si>
+    <t>리스트를 표시할 수 있다.</t>
+  </si>
+  <si>
+    <t>스토리 리스트</t>
+  </si>
+  <si>
+    <t>대표 이미지,  제목, 최종 수정 일(XXXX년 XX월 XX일 XX시 XX분 XX초</t>
+  </si>
+  <si>
+    <t>대표 이미지,  제목, 최종 수정 일(XXXX년 XX월 XX일 XX시 XX분 XX초) 표시</t>
+  </si>
+  <si>
+    <t xml:space="preserve">스토리는 XXXX년 XX월 을 기준으로 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">스토리는 "XXXX년 XX월" 을 기준으로 </t>
+  </si>
+  <si>
+    <t>결과</t>
+  </si>
+  <si>
+    <t>상세</t>
+  </si>
+  <si>
+    <t>XX초 표시 안됨. Text Size 변경 필요</t>
+  </si>
+  <si>
+    <t>스토리는 "XXXX년 XX월" 을 기준으로 그룹</t>
+  </si>
+  <si>
+    <t>스토리는 "XXXX년 XX월" 을 기준으로 그룹화하여 표시</t>
+  </si>
+  <si>
+    <t>각 그룹 헤더는 스토리 개수를 표시한다.</t>
+  </si>
+  <si>
+    <t>그룹 헤더 클릭 시 해당 월의 스토리가 펼쳐져서 보여진다.</t>
+  </si>
+  <si>
+    <t>리스트 삭제</t>
+  </si>
+  <si>
+    <t>리스트 표시</t>
+  </si>
+  <si>
+    <t>기능</t>
+  </si>
+  <si>
+    <t>Swipe를 이용해 스토리를 삭제할 수 있다.</t>
+  </si>
+  <si>
+    <t>현재 개발 중.</t>
+  </si>
+  <si>
+    <t>Long click을 통해 스토리를 삭제 할 수 있다. Snackbar를 통해 삭제 의사 확인 후 진행.</t>
+  </si>
+  <si>
+    <t>최종 삭제되었는지 확인</t>
+  </si>
+  <si>
+    <t>카메라, Edit 등의 내부 화면이나 Home을 통해 외부화면으로 이동 후 재진입 시에도 스토리 삭제가 정상적으로 되었는지 확인</t>
+  </si>
+  <si>
+    <t>스토리 삭제</t>
+  </si>
+  <si>
+    <t>새로운 스토리 추가 시에 정상적으로 추가되는 지 확인</t>
+  </si>
+  <si>
+    <t>새로운 스토리 추가 시에 정상적으로 추가되는지 확인</t>
+  </si>
+  <si>
+    <t>카메라</t>
+  </si>
+  <si>
+    <t>카메라 캡쳐</t>
+  </si>
+  <si>
+    <t>사진 촬영</t>
+  </si>
+  <si>
+    <t>진입 후 사진을 찍지 않고 완료 버튼이 동작하는지 확인한다.
+(동작하지 않는 것이 정상)</t>
+  </si>
+  <si>
+    <t>사진없이도 스토리를 쓸수 있으므로 고려해봐야 함.</t>
+  </si>
+  <si>
+    <t>사진없이도 스토리를 쓸수 있으므로 고려해봐야 함.
+나중에 추가할 수 있는 기능도 고려해야 함.</t>
+  </si>
+  <si>
+    <t>다른 화면으로 진입 후 시스템 카메라 폰이 정상적으로 동작하는지 확인</t>
+  </si>
+  <si>
+    <t>진입 후 사진을 찍지 않고 종료 버튼이 동작하는지 확인한다.
+(동작하지 않는 것이 정상)</t>
+  </si>
+  <si>
+    <t>사진 촬영 -&gt; 종료 -&gt; 스토리 생성 화면에 진입 -&gt; back  입력 시 사진 개수가 그대로 잘 표시되는지 확인</t>
+  </si>
+  <si>
+    <t>생성/편집</t>
+  </si>
+  <si>
+    <t>스토리 생성/편집</t>
+  </si>
+  <si>
+    <t>스토리 생성</t>
+  </si>
+  <si>
+    <t>사진 촬영 후 진입 시 사진 개수가 정상적으로 표시되는지 확인</t>
+  </si>
+  <si>
+    <t>사진 촬영 후 진입 시 사진 및 개수가 정상적으로 표시되는지 확인</t>
+  </si>
+  <si>
+    <t>제목은 1줄 입력되는지 확인</t>
+  </si>
+  <si>
+    <t>18자로 limit을 걸어놨으나 필요하면 더 늘릴 수 있음</t>
+  </si>
+  <si>
+    <t>메모는 Multi line 지원되는지 확인</t>
+  </si>
+  <si>
+    <t>생성된 스토리가 스토리 리스트 화면으로 이동후에도 정상적으로 표시되는 지 확인</t>
+  </si>
+  <si>
+    <t>스토리 편집</t>
+  </si>
+  <si>
+    <t>생성 혹은 이전 편집 시 입력한 값이 정상적으로 표시되는지 확인</t>
+  </si>
+  <si>
+    <t>Thumbnail 선택 시 popup으로 확대 사진이 표시되는지 확인</t>
+  </si>
+  <si>
+    <t>검색</t>
+  </si>
+  <si>
+    <t>검색 버튼을 눌러 특정 단어를 입력 후 검색 시 제목/메모 기준으로 검색되는지 확인</t>
+  </si>
+  <si>
+    <t>검색 취소 시 리스트가 원복되는지 확인</t>
+  </si>
+  <si>
+    <t>한글자 입력 시 마다 검색되어야 할지 고민..</t>
+  </si>
+  <si>
+    <t>Camera 제어 부분 Presenter로 코드 이동</t>
+  </si>
+  <si>
+    <t>`</t>
   </si>
 </sst>
 </file>
@@ -192,7 +360,7 @@
       <color rgb="FF7F7F7F"/>
     </font>
   </fonts>
-  <fills count="33">
+  <fills count="56">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -356,8 +524,123 @@
         <fgColor theme="9" tint="0.399980"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFDEEBF7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFBE5D6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFEDEDED"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFF2CC"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFDAE3F3"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFE2F0D9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFBDD7EE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF8CBAD"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFDBDBDB"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFE699"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFB4C7E7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC5E0B4"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF9DC3E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF4B183"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC9C9C9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFD966"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF8FAADC"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA9D18E"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF5B9BD5"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFED7D31"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF4472C4"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF70AD47"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="10">
+  <borders count="19">
     <border>
       <left/>
       <right/>
@@ -475,6 +758,99 @@
       <diagonal style="none">
         <color rgb="FF000000"/>
       </diagonal>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <top style="thin">
+        <color rgb="FF5B9BD5"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF5B9BD5"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <bottom style="thick">
+        <color rgb="FF5B9BD5"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <bottom style="thick">
+        <color rgb="FFACCCEA"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <bottom style="medium">
+        <color rgb="FF9DC3E6"/>
+      </bottom>
+      <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="49">
@@ -528,8 +904,159 @@
     <xf numFmtId="0" fontId="18" fillId="32" borderId="0" applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="52">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="fill" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="fill" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="16" fillId="7" borderId="0" xfId="22" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="8" borderId="0" xfId="23" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="6" borderId="0" xfId="21" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="9">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="10" xfId="17" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="8" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="48">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="5" borderId="12" xfId="18" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="13" xfId="19" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="10" xfId="15" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="14" xfId="16" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="15" xfId="20" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="10">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="16" xfId="11" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="17" xfId="12" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="18" xfId="13" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="14">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="25" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="29" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="35" borderId="0" xfId="33" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="36" borderId="0" xfId="37" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="37" borderId="0" xfId="41" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="38" borderId="0" xfId="45" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="39" borderId="0" xfId="26" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="40" borderId="0" xfId="30" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="41" borderId="0" xfId="34" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="42" borderId="0" xfId="38" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="43" borderId="0" xfId="42" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="44" borderId="0" xfId="46" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="45" borderId="0" xfId="27" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="46" borderId="0" xfId="31" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="47" borderId="0" xfId="35" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="48" borderId="0" xfId="39" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="49" borderId="0" xfId="43" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="50" borderId="0" xfId="47" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="51" borderId="0" xfId="24" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="52" borderId="0" xfId="28" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="5" borderId="0" xfId="32" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="53" borderId="0" xfId="36" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="54" borderId="0" xfId="40" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="55" borderId="0" xfId="44" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="3" applyNumberFormat="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" xfId="4" applyNumberFormat="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="7" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="5" fontId="0" fillId="0" borderId="0" xfId="5" applyNumberFormat="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -851,10 +1378,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A2:C21"/>
+  <dimension ref="A2:C24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.500000"/>
@@ -872,16 +1399,16 @@
       </c>
     </row>
     <row r="3" spans="1:3">
-      <c r="B3" s="0" t="s">
+      <c r="B3" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="0" t="s">
+      <c r="C3" s="8" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="4" spans="1:3">
       <c r="B4" s="0" t="s">
-        <v>9</v>
+        <v>72</v>
       </c>
     </row>
     <row r="5" spans="1:3">
@@ -893,18 +1420,18 @@
       <c r="A8" s="0" t="s">
         <v>3</v>
       </c>
-      <c r="B8" s="0" t="s">
+      <c r="B8" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="C8" s="0" t="s">
+      <c r="C8" s="8" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="9" spans="1:3">
-      <c r="B9" s="0" t="s">
+      <c r="B9" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="C9" s="0" t="s">
+      <c r="C9" s="8" t="s">
         <v>17</v>
       </c>
     </row>
@@ -913,14 +1440,19 @@
         <v>15</v>
       </c>
     </row>
+    <row r="11" spans="1:3">
+      <c r="B11" s="0" t="s">
+        <v>73</v>
+      </c>
+    </row>
     <row r="14" spans="1:3">
       <c r="A14" s="0" t="s">
         <v>13</v>
       </c>
-      <c r="B14" s="0" t="s">
+      <c r="B14" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="C14" s="0" t="s">
+      <c r="C14" s="8" t="s">
         <v>17</v>
       </c>
     </row>
@@ -935,6 +1467,14 @@
       </c>
       <c r="B21" s="0" t="s">
         <v>8</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2">
+      <c r="A24" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="B24" s="0" t="s">
+        <v>20</v>
       </c>
     </row>
   </sheetData>
@@ -946,14 +1486,174 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+  <dimension ref="B1:E28"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.500000"/>
-  <sheetData/>
+  <cols>
+    <col min="2" max="2" width="16.50500011" customWidth="1" outlineLevel="0"/>
+    <col min="3" max="3" width="22.50499916" customWidth="1" outlineLevel="0"/>
+    <col min="4" max="4" style="3" width="55.50500107" customWidth="1" outlineLevel="0"/>
+    <col min="5" max="5" width="46.00500107" customWidth="1" outlineLevel="0"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:5" ht="17.300000">
+      <c r="C1" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="E1" s="0" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="2" spans="2:5" ht="34.050000">
+      <c r="B2" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="C2" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="E2" s="0" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="3" spans="2:5" ht="17.300000">
+      <c r="D3" s="3" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="4" spans="2:5" ht="17.300000">
+      <c r="D4" s="3" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="5" spans="2:5" ht="17.300000">
+      <c r="D5" s="3" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="6" spans="2:5" ht="17.300000">
+      <c r="D6" s="3" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="7" spans="2:5"/>
+    <row r="8" spans="2:5"/>
+    <row r="9" spans="2:5" ht="17.300000">
+      <c r="C9" s="0" t="s">
+        <v>44</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="E9" s="0" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="10" spans="2:5" ht="34.050000">
+      <c r="D10" s="3" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="11" spans="2:5" ht="34.050000">
+      <c r="D11" s="3" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="12" spans="2:5"/>
+    <row r="13" spans="2:5" ht="34.050000">
+      <c r="C13" s="0" t="s">
+        <v>68</v>
+      </c>
+      <c r="D13" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="E13" s="0" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="14" spans="2:5" ht="17.300000">
+      <c r="D14" s="3" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="15" spans="2:5"/>
+    <row r="16" spans="2:5"/>
+    <row r="18" spans="2:5" ht="34.050000">
+      <c r="B18" s="0" t="s">
+        <v>47</v>
+      </c>
+      <c r="C18" s="0" t="s">
+        <v>49</v>
+      </c>
+      <c r="D18" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="E18" s="3" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="19" spans="2:5" ht="34.050000">
+      <c r="D19" s="3" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="20" spans="2:5" ht="34.050000">
+      <c r="D20" s="3" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="22" spans="2:5" ht="17.300000">
+      <c r="B22" s="0" t="s">
+        <v>57</v>
+      </c>
+      <c r="C22" s="0" t="s">
+        <v>58</v>
+      </c>
+      <c r="D22" s="3" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="23" spans="2:5" ht="17.300000">
+      <c r="D23" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="E23" s="0" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="24" spans="2:5" ht="17.300000">
+      <c r="D24" s="3" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="25" spans="2:5" ht="34.050000">
+      <c r="D25" s="3" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="27" spans="2:5" ht="17.300000">
+      <c r="C27" s="0" t="s">
+        <v>65</v>
+      </c>
+      <c r="D27" s="3" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="28" spans="2:5" ht="17.300000">
+      <c r="D28" s="3" t="s">
+        <v>67</v>
+      </c>
+    </row>
+  </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.70" right="0.70" top="0.75" bottom="0.75" header="0.30" footer="0.30"/>
   <pageSetup paperSize="9" orientation="portrait"/>

</xml_diff>